<commit_message>
First part developmment threading, add class
</commit_message>
<xml_diff>
--- a/optimisation/timing.xlsx
+++ b/optimisation/timing.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D20D25A-30A5-4D69-B5B8-676F77B64B81}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BA48874-FA60-4E46-819F-5A54A3C40425}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="18">
   <si>
     <t>TabStats_V01</t>
   </si>
@@ -68,6 +68,12 @@
   </si>
   <si>
     <t>14.083</t>
+  </si>
+  <si>
+    <t>Branche multithread</t>
+  </si>
+  <si>
+    <t>FAIRE UNE COURBE!!!</t>
   </si>
 </sst>
 </file>
@@ -83,15 +89,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -99,15 +111,29 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -139,8 +165,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{82584656-22BE-4D40-A6C3-8637B22950DE}" name="Tableau1" displayName="Tableau1" ref="A1:G7" totalsRowShown="0">
-  <autoFilter ref="A1:G7" xr:uid="{AD5B8D72-9EEE-45EC-90A4-50F93DAE5D46}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{82584656-22BE-4D40-A6C3-8637B22950DE}" name="Tableau1" displayName="Tableau1" ref="A1:G8" totalsRowShown="0">
+  <autoFilter ref="A1:G8" xr:uid="{AD5B8D72-9EEE-45EC-90A4-50F93DAE5D46}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{AAF3DC49-0ED7-425B-9305-FB8F89335F33}" name="TabStats_Versions"/>
     <tableColumn id="2" xr3:uid="{6357748C-05AF-40FC-B3EF-E5264A013C18}" name="Fx"/>
@@ -417,10 +443,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -598,6 +624,22 @@
         <v>15504</v>
       </c>
     </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="G8" s="1"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Refactor code for threading (bugged)
</commit_message>
<xml_diff>
--- a/optimisation/timing.xlsx
+++ b/optimisation/timing.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BA48874-FA60-4E46-819F-5A54A3C40425}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A572EAFE-4406-4F02-96CB-62A7760F0C58}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2805" yWindow="2805" windowWidth="21600" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="19">
   <si>
     <t>TabStats_V01</t>
   </si>
@@ -74,6 +74,9 @@
   </si>
   <si>
     <t>FAIRE UNE COURBE!!!</t>
+  </si>
+  <si>
+    <t>635723.112</t>
   </si>
 </sst>
 </file>
@@ -446,7 +449,7 @@
   <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -625,10 +628,27 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="G8" s="1"/>
+      <c r="A8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" s="1">
+        <v>10</v>
+      </c>
+      <c r="D8" s="1">
+        <v>30</v>
+      </c>
+      <c r="E8" s="1">
+        <v>2</v>
+      </c>
+      <c r="F8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G8" s="1">
+        <v>435</v>
+      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">

</xml_diff>

<commit_message>
Add timing for F2 function
</commit_message>
<xml_diff>
--- a/optimisation/timing.xlsx
+++ b/optimisation/timing.xlsx
@@ -3,15 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{064C0C92-B8D0-4D44-A300-2076BFDFC11B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6527CC46-599E-43F8-8D1A-F20CD21247E9}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3495" yWindow="3495" windowWidth="21600" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16905" yWindow="2400" windowWidth="21600" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -21,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="24">
   <si>
     <t>TabStats_V01</t>
   </si>
@@ -44,9 +43,6 @@
     <t>Timing_Exec</t>
   </si>
   <si>
-    <t>obj par groupe</t>
-  </si>
-  <si>
     <t>Nbre de combin</t>
   </si>
   <si>
@@ -81,6 +77,21 @@
   </si>
   <si>
     <t>Regarder pourquoi ajouter un fichier init.py</t>
+  </si>
+  <si>
+    <t>TabStats_V02</t>
+  </si>
+  <si>
+    <t>1.002 sec</t>
+  </si>
+  <si>
+    <t>2.673</t>
+  </si>
+  <si>
+    <t>Obj par groupe</t>
+  </si>
+  <si>
+    <t>22.687</t>
   </si>
 </sst>
 </file>
@@ -145,7 +156,19 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="8">
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -177,11 +200,27 @@
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{AAF3DC49-0ED7-425B-9305-FB8F89335F33}" name="TabStats_Versions"/>
     <tableColumn id="2" xr3:uid="{6357748C-05AF-40FC-B3EF-E5264A013C18}" name="Fx"/>
-    <tableColumn id="6" xr3:uid="{2743E559-8066-470B-A33E-56AF0E905B49}" name="Essais" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{C5BA6E02-DC0B-4649-9495-88C602EA5052}" name="Colonnes" dataDxfId="2"/>
-    <tableColumn id="7" xr3:uid="{341402B5-65D1-4310-B96A-81266B86A263}" name="obj par groupe" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{2743E559-8066-470B-A33E-56AF0E905B49}" name="Essais" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{C5BA6E02-DC0B-4649-9495-88C602EA5052}" name="Colonnes" dataDxfId="6"/>
+    <tableColumn id="7" xr3:uid="{341402B5-65D1-4310-B96A-81266B86A263}" name="Obj par groupe" dataDxfId="5"/>
     <tableColumn id="3" xr3:uid="{B3C81405-2D43-4E38-90D9-35D2EC04D185}" name="Timing_Exec"/>
-    <tableColumn id="8" xr3:uid="{E3F123D0-3CA3-4D6A-A46D-2CBB505151AE}" name="Nbre de combin" dataDxfId="0"/>
+    <tableColumn id="8" xr3:uid="{E3F123D0-3CA3-4D6A-A46D-2CBB505151AE}" name="Nbre de combin" dataDxfId="4"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{1C124662-C0F1-4208-8F15-882F7AC8B086}" name="Tableau14" displayName="Tableau14" ref="A11:G18" totalsRowShown="0">
+  <autoFilter ref="A11:G18" xr:uid="{D43116E3-3857-482A-B770-28A52E4C76D2}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{25480CA7-329B-4002-93ED-FA1395E9E080}" name="TabStats_Versions"/>
+    <tableColumn id="2" xr3:uid="{9FC70F22-7E64-4084-826C-C391CB219CE4}" name="Fx"/>
+    <tableColumn id="6" xr3:uid="{2BC9CE2E-F5CF-4C61-9519-A746394D7B6B}" name="Essais" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{91E9FD73-0C76-4232-AC1A-9B08C6DC1DAC}" name="Colonnes" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{C833F70F-D7E9-4FE3-A92D-88E521F9171B}" name="Obj par groupe" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{27A5016C-D5C7-400A-AAF7-F8852B654F5F}" name="Timing_Exec"/>
+    <tableColumn id="8" xr3:uid="{D770F57D-C0CC-446B-AC38-08E5CA4555B5}" name="Nbre de combin" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -450,10 +489,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:I27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -472,7 +511,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C1" t="s">
         <v>3</v>
@@ -481,13 +520,13 @@
         <v>4</v>
       </c>
       <c r="E1" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="F1" t="s">
         <v>6</v>
       </c>
       <c r="G1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -507,7 +546,7 @@
         <v>2</v>
       </c>
       <c r="F2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G2" s="1">
         <v>45</v>
@@ -533,7 +572,7 @@
         <v>5</v>
       </c>
       <c r="F3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G3" s="1">
         <v>252</v>
@@ -556,7 +595,7 @@
         <v>2</v>
       </c>
       <c r="F4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G4" s="1">
         <v>105</v>
@@ -579,7 +618,7 @@
         <v>5</v>
       </c>
       <c r="F5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G5" s="1">
         <v>3003</v>
@@ -602,7 +641,7 @@
         <v>2</v>
       </c>
       <c r="F6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G6" s="1">
         <v>190</v>
@@ -625,7 +664,7 @@
         <v>5</v>
       </c>
       <c r="F7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G7" s="1">
         <v>15504</v>
@@ -648,32 +687,217 @@
         <v>2</v>
       </c>
       <c r="F8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G8" s="1">
         <v>435</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>16</v>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11" t="s">
+        <v>4</v>
+      </c>
+      <c r="E11" t="s">
+        <v>22</v>
+      </c>
+      <c r="F11" t="s">
+        <v>6</v>
+      </c>
+      <c r="G11" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>17</v>
+      <c r="A12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" s="1">
+        <v>10</v>
+      </c>
+      <c r="D12" s="1">
+        <v>10</v>
+      </c>
+      <c r="E12" s="1">
+        <v>2</v>
+      </c>
+      <c r="F12" t="s">
+        <v>20</v>
+      </c>
+      <c r="G12" s="1">
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>19</v>
+        <v>0</v>
+      </c>
+      <c r="B13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13" s="1">
+        <v>10</v>
+      </c>
+      <c r="D13" s="1">
+        <v>10</v>
+      </c>
+      <c r="E13" s="1">
+        <v>5</v>
+      </c>
+      <c r="F13" t="s">
+        <v>21</v>
+      </c>
+      <c r="G13" s="1">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" s="1">
+        <v>10</v>
+      </c>
+      <c r="D14" s="1">
+        <v>15</v>
+      </c>
+      <c r="E14" s="1">
+        <v>2</v>
+      </c>
+      <c r="F14" t="s">
+        <v>23</v>
+      </c>
+      <c r="G14" s="1">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" s="1">
+        <v>10</v>
+      </c>
+      <c r="D15" s="1">
+        <v>15</v>
+      </c>
+      <c r="E15" s="1">
+        <v>5</v>
+      </c>
+      <c r="F15" t="s">
+        <v>13</v>
+      </c>
+      <c r="G15" s="1">
+        <v>3003</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" s="1">
+        <v>10</v>
+      </c>
+      <c r="D16" s="1">
+        <v>20</v>
+      </c>
+      <c r="E16" s="1">
+        <v>2</v>
+      </c>
+      <c r="F16" t="s">
+        <v>12</v>
+      </c>
+      <c r="G16" s="1">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" t="s">
+        <v>2</v>
+      </c>
+      <c r="C17" s="1">
+        <v>10</v>
+      </c>
+      <c r="D17" s="1">
+        <v>20</v>
+      </c>
+      <c r="E17" s="1">
+        <v>5</v>
+      </c>
+      <c r="F17" t="s">
+        <v>11</v>
+      </c>
+      <c r="G17" s="1">
+        <v>15504</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" t="s">
+        <v>2</v>
+      </c>
+      <c r="C18" s="1">
+        <v>10</v>
+      </c>
+      <c r="D18" s="1">
+        <v>30</v>
+      </c>
+      <c r="E18" s="1">
+        <v>2</v>
+      </c>
+      <c r="F18" t="s">
+        <v>17</v>
+      </c>
+      <c r="G18" s="1">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
-  <tableParts count="1">
+  <tableParts count="2">
     <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
threads on F2 do not get combin list, this function has moved to now file
</commit_message>
<xml_diff>
--- a/optimisation/timing.xlsx
+++ b/optimisation/timing.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6527CC46-599E-43F8-8D1A-F20CD21247E9}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B2BA983-E56F-45A5-839D-A347232CF78B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="16905" yWindow="2400" windowWidth="21600" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="25">
   <si>
     <t>TabStats_V01</t>
   </si>
@@ -82,16 +82,19 @@
     <t>TabStats_V02</t>
   </si>
   <si>
-    <t>1.002 sec</t>
-  </si>
-  <si>
-    <t>2.673</t>
-  </si>
-  <si>
     <t>Obj par groupe</t>
   </si>
   <si>
-    <t>22.687</t>
+    <t>0.724 sec</t>
+  </si>
+  <si>
+    <t>2.473</t>
+  </si>
+  <si>
+    <t>36.197</t>
+  </si>
+  <si>
+    <t>12.469</t>
   </si>
 </sst>
 </file>
@@ -520,7 +523,7 @@
         <v>4</v>
       </c>
       <c r="E1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F1" t="s">
         <v>6</v>
@@ -712,7 +715,7 @@
         <v>4</v>
       </c>
       <c r="E11" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F11" t="s">
         <v>6</v>
@@ -738,7 +741,7 @@
         <v>2</v>
       </c>
       <c r="F12" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G12" s="1">
         <v>45</v>
@@ -761,7 +764,7 @@
         <v>5</v>
       </c>
       <c r="F13" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G13" s="1">
         <v>252</v>
@@ -784,7 +787,7 @@
         <v>2</v>
       </c>
       <c r="F14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G14" s="1">
         <v>105</v>
@@ -807,7 +810,7 @@
         <v>5</v>
       </c>
       <c r="F15" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="G15" s="1">
         <v>3003</v>

</xml_diff>